<commit_message>
update behavioural term upload jobs
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/Calibration/CalibrationInput_EAD_Behavioural_Terms.xlsx
+++ b/angular/src/assets/sampleFiles/Calibration/CalibrationInput_EAD_Behavioural_Terms.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryemitan\Desktop\Dev\ECL Automation\ETI\App\Sample Uploads\Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryemitan\Desktop\Dev\ECL Automation\ETI\App\ETI_ECL_Engine\angular\src\assets\sampleFiles\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95404FCC-926D-49C1-9724-CC43AE545F97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9E587D-B42B-449C-8794-F6F8B9995222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="900" windowWidth="18330" windowHeight="11205" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="27" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="33">
   <si>
     <t>Customer_No</t>
   </si>
@@ -78,21 +78,6 @@
   </si>
   <si>
     <t>Restructure_End_Date</t>
-  </si>
-  <si>
-    <t>Assumption_NonExpired</t>
-  </si>
-  <si>
-    <t>Freq_NonExpired</t>
-  </si>
-  <si>
-    <t>Assumption_Expired</t>
-  </si>
-  <si>
-    <t>Freq_Expired</t>
-  </si>
-  <si>
-    <t>Comment</t>
   </si>
   <si>
     <t>30001552</t>
@@ -154,7 +139,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -624,7 +609,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4"/>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="7"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
@@ -648,7 +633,7 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
@@ -982,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B1E5E2-FB3A-4804-B949-E2061B45DF3F}">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,14 +990,9 @@
     <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1058,40 +1038,25 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E2" s="3">
         <v>42643</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G2" s="6">
         <v>0</v>
@@ -1109,32 +1074,32 @@
         <v>41137</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3">
         <v>42735</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
@@ -1152,32 +1117,32 @@
         <v>41137</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3">
         <v>42825</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G4" s="6">
         <v>0</v>
@@ -1195,32 +1160,32 @@
         <v>42122</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3">
         <v>42916</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G5" s="6">
         <v>0</v>
@@ -1238,32 +1203,32 @@
         <v>41137</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3">
         <v>43008</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G6" s="6">
         <v>0</v>
@@ -1281,32 +1246,32 @@
         <v>41137</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3">
         <v>42825</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -1324,32 +1289,32 @@
         <v>42091</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E8" s="3">
         <v>42916</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G8" s="6">
         <v>0</v>
@@ -1367,32 +1332,32 @@
         <v>42735</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E9" s="3">
         <v>43008</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G9" s="6">
         <v>0</v>
@@ -1410,32 +1375,32 @@
         <v>42735</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E10" s="3">
         <v>42825</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G10" s="6">
         <v>0</v>
@@ -1453,32 +1418,32 @@
         <v>41026</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E11" s="3">
         <v>42916</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G11" s="6">
         <v>0</v>
@@ -1496,32 +1461,32 @@
         <v>41029</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E12" s="3">
         <v>43008</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G12" s="6">
         <v>0</v>
@@ -1539,32 +1504,32 @@
         <v>41029</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E13" s="3">
         <v>43100</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -1582,32 +1547,32 @@
         <v>41029</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E14" s="3">
         <v>43190</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -1625,32 +1590,32 @@
         <v>43031</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E15" s="3">
         <v>42643</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G15" s="6">
         <v>0</v>
@@ -1668,32 +1633,32 @@
         <v>41029</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E16" s="3">
         <v>42735</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G16" s="6">
         <v>0</v>
@@ -1711,32 +1676,32 @@
         <v>41029</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3">
         <v>43100</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G17" s="6">
         <v>0</v>
@@ -1754,32 +1719,32 @@
         <v>43131</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E18" s="3">
         <v>43190</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G18" s="6">
         <v>0</v>
@@ -1797,10 +1762,10 @@
         <v>43190</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>

</xml_diff>

<commit_message>
update calibration sample templates, data readers & data exporters
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/Calibration/CalibrationInput_EAD_Behavioural_Terms.xlsx
+++ b/angular/src/assets/sampleFiles/Calibration/CalibrationInput_EAD_Behavioural_Terms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryemitan\Desktop\Dev\ECL Automation\ETI\App\ETI_ECL_Engine\angular\src\assets\sampleFiles\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9E587D-B42B-449C-8794-F6F8B9995222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D51133A-D494-41FB-A989-429A19C8291F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -626,7 +626,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
@@ -636,6 +636,8 @@
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1 2" xfId="1" xr:uid="{5619AD69-9119-47E2-B6B7-2C8EA97AB0E0}"/>
@@ -969,27 +971,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B1E5E2-FB3A-4804-B949-E2061B45DF3F}">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -1011,13 +1012,13 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
@@ -1032,10 +1033,10 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="8" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
serial on calibration data
</commit_message>
<xml_diff>
--- a/angular/src/assets/sampleFiles/Calibration/CalibrationInput_EAD_Behavioural_Terms.xlsx
+++ b/angular/src/assets/sampleFiles/Calibration/CalibrationInput_EAD_Behavioural_Terms.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryemitan\Desktop\Dev\ECL Automation\ETI\App\ETI_ECL_Engine\angular\src\assets\sampleFiles\Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PwC\Projects\SourceCode\Firs_9_ECL\FrontEnd\angular\src\assets\sampleFiles\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D51133A-D494-41FB-A989-429A19C8291F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8344262C-8B3D-4AE3-8969-4AAA0EA6D0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="27" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -972,7 +970,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>